<commit_message>
Update Literature Matrix UU 2022.xlsx
</commit_message>
<xml_diff>
--- a/LITERATURE REVIEW/Literature Matrix UU 2022.xlsx
+++ b/LITERATURE REVIEW/Literature Matrix UU 2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mwang002\Documents\GitHub\Renewable_Energy_Integration\LITERATURE REVIEW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agrippina Mwangi\Documents\GitHub\Renewable_Energy_Integration\LITERATURE REVIEW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C43AD3F-982F-42F7-9803-AA21BA60B4FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52691A55-9EDA-487E-9CD5-295CF6B59354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="768" windowWidth="11280" windowHeight="8964" xr2:uid="{497C0ADB-D672-4D47-81E2-3B9010C22FDB}"/>
+    <workbookView xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="8964" xr2:uid="{497C0ADB-D672-4D47-81E2-3B9010C22FDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Month 1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Title/Author</t>
   </si>
@@ -151,6 +151,45 @@
   </si>
   <si>
     <t>A framework for wide area monitoring and control systems interoperability and cybersecurity analysis</t>
+  </si>
+  <si>
+    <t>Anam Sajid, Haider Abbas, Kashif saleem</t>
+  </si>
+  <si>
+    <t>Cloud-assisted IoT based SCADA systems security: A review of the state of the art and future challenges</t>
+  </si>
+  <si>
+    <t>The IoT-cloud based SCADA ICS faces vulnerabilities as it is integrated with underlying legacy systems. Some of these vulnerabilities are as a result of the weak (insecure) communication protocols - Modbus, IEC 61850, and CI systems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The survey paper explores the different kinds of vulnerabilities faced since the adoption of the networked and the IoT cloud based SCADA system approaches. The paper reviews the different attacks that have hit several organizations siting CIA for security risk analysis. </t>
+  </si>
+  <si>
+    <t>SCADA systems are susceptible to vulnerabilities during communication and at the CI layer as well since most Industrial applications use commercial cloud services. This survey equally presents case scenarios of different threats: eavesdropping, man-in-the-middle attacks, data corruption owing to lack of proper security controls</t>
+  </si>
+  <si>
+    <r>
+      <t>This paper is quite important as it addresses the differen threats. It reviews the chronological advancement in the design and implementation of SCADA systems. The paper discusses the vulnerabilities of communication layer (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>overview</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">) and proposes the use of multiple layers of security as well as redundancy as a preventative measure. </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -521,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99C6CAC5-4A2C-4BDD-A220-11C3DA4654B6}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
@@ -651,6 +690,26 @@
         <v>34</v>
       </c>
     </row>
+    <row r="7" spans="1:8" ht="211.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>